<commit_message>
- FIX: Fixed issue with wrong formula in germplasm mcpd template.
</commit_message>
<xml_diff>
--- a/germplasm/germplasm-mcpd.xlsx
+++ b/germplasm/germplasm-mcpd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\other\germinate-data-templates\germplasm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45228130-5E5A-4992-9369-43312EE24963}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD13D59-40A5-47B9-9653-3EB857286E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="2" r:id="rId1"/>
@@ -1076,7 +1076,7 @@
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="SPECIES"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="SPAUTHOR"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="SUBTAXA" dataDxfId="16">
-      <calculatedColumnFormula>IF(AND(NOT(ISBLANK(JS)), NOT(ISBLANK(K2))), J2&amp;K2, "")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(AND(NOT(ISBLANK(J2)), NOT(ISBLANK(K2))), J2&amp;K2, "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SUBTAUTHOR"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="CROPNAME"/>
@@ -1702,7 +1702,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="L2" t="str">
-        <f>IF(AND(NOT(ISBLANK(JS)), NOT(ISBLANK(K2))), J2&amp;K2, "")</f>
+        <f>IF(AND(NOT(ISBLANK(J2)), NOT(ISBLANK(K2))), J2&amp;K2, "")</f>
         <v/>
       </c>
       <c r="AU2" s="19" t="s">

</xml_diff>

<commit_message>
- CHG: Small updates to docs.
</commit_message>
<xml_diff>
--- a/germplasm/germplasm-mcpd.xlsx
+++ b/germplasm/germplasm-mcpd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\germplasm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA32E6D8-97EE-4E4B-8765-E8CDA1ECC431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ACAD5C-E491-43AB-AF3A-D00C214DB1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15900" yWindow="4185" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="257">
   <si>
     <t>PUID</t>
   </si>
@@ -1361,8 +1361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table22" displayName="Table22" ref="A1:AO9" totalsRowShown="0">
-  <tableColumns count="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table22" displayName="Table22" ref="A1:AQ9" totalsRowShown="0">
+  <tableColumns count="43">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PUID" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="INSTCODE" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="ACCENUMB" dataDxfId="13"/>
@@ -1404,6 +1404,8 @@
     <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="STORAGE"/>
     <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="MLSSTAT"/>
     <tableColumn id="41" xr3:uid="{00000000-0010-0000-0100-000029000000}" name="REMARKS"/>
+    <tableColumn id="42" xr3:uid="{C1D72FCB-FA8A-4239-9D0A-2DC9C4F96305}" name="Entity type"/>
+    <tableColumn id="43" xr3:uid="{B3B1976D-371C-4399-B242-A9C7A73A0848}" name="Entity parent ACCENUMB"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1924,8 +1926,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AU4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AP1:AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2234,7 @@
   <dimension ref="A1:A67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,10 +2555,10 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AO21"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AO9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,9 +2604,11 @@
     <col min="39" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="9" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.85546875" customWidth="1"/>
+    <col min="43" max="43" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2728,8 +2732,14 @@
       <c r="AO1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP1" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>204</v>
       </c>
@@ -2841,8 +2851,12 @@
       <c r="AN2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP2" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ2" s="11"/>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>205</v>
       </c>
@@ -2951,8 +2965,11 @@
       <c r="AN3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP3" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>206</v>
       </c>
@@ -3061,8 +3078,11 @@
       <c r="AN4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP4" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>207</v>
       </c>
@@ -3174,8 +3194,11 @@
       <c r="AN5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP5" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>208</v>
       </c>
@@ -3284,8 +3307,11 @@
       <c r="AN6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP6" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>209</v>
       </c>
@@ -3394,8 +3420,11 @@
       <c r="AN7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP7" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>210</v>
       </c>
@@ -3504,8 +3533,11 @@
       <c r="AN8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP8" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>211</v>
       </c>
@@ -3616,6 +3648,9 @@
       </c>
       <c r="AN9">
         <v>0</v>
+      </c>
+      <c r="AP9" s="11" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
@@ -3624,7 +3659,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="41">
+  <dataValidations count="42">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Remarks" prompt="Add notes or elaborate on descriptors with value 99 or 999 (=Other).Prefix remarks with the field name they refer to and a colon without space, e.g. COLLSRC:riverside. Distinct remarks referring to different fields are separated by semicolon without space" sqref="AO1" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="MLS Status Of Accession" prompt="Status of the accession with regards to Multilateral System (MLS) of the ITPGRFA. 0 - No (not included); 1 - Yes (included); 99 - Other (elaborate in REMARKS field, e.g. 'under development')._x000a_Leave empty if status is not known. " sqref="AN1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Type Of Germplasm Storage" prompt="If germplasm is maintained under different types of storage, multiple choices are allowed, separated by a semicolon (e.g. 20;30). (Refer to FAO/IPGRI Genebank Standards 1994 for details on storage type.) For details see tab 'INFO'." sqref="AM1" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
@@ -3666,6 +3701,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Accession Number" prompt="This is the unique identifier for accessions within a genebank, and is assigned when a sample is entered into the genebank collection (e.g. ‘PI 113869’)." sqref="C1" xr:uid="{00000000-0002-0000-0400-000026000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Institute Code" prompt="Code of the institute where the accession is maintained. Codes consist of 3-letter ISO 3166 country coe of the country where the institute is located plus a number (e.g. COL001)._x000a_Current set of institute codes is available from http://www.fao.org/wiews." sqref="B1" xr:uid="{00000000-0002-0000-0400-000027000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Persistent Unique Identifier" prompt="Any persistent, unique identifier assigned to the accession so it can be unambiguously referenced at the global level and the information associated with it harvested through automated means. Report one PUID for each accession._x000a_" sqref="A1" xr:uid="{00000000-0002-0000-0400-000028000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="AP1:AP1048576" xr:uid="{CE09E684-79F3-4DAD-B54D-8023BFF3948B}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>